<commit_message>
Verifify email & Docs & cities.txt
</commit_message>
<xml_diff>
--- a/GetAgent Docs/SAD/פרטיי חומרה ותוכנה וממשקים פיזיים.xlsx
+++ b/GetAgent Docs/SAD/פרטיי חומרה ותוכנה וממשקים פיזיים.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\www\Self Projects\GetAgent\GetAgent Docs\SAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EED934-BD2D-4CA0-B0B1-12F8099A58DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F0B3A5-D1F3-44A3-A242-33A246301811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FBA8AAB7-FCC3-459F-BBC2-C8F7327FEB60}"/>
   </bookViews>
@@ -199,7 +199,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,46 +248,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67811B3B-04EB-45B1-B0D3-FA3A8E860648}">
   <dimension ref="C3:K34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -615,276 +615,276 @@
     <col min="3" max="3" width="12.3984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.796875" style="2"/>
-    <col min="7" max="7" width="13" style="12" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="12" customWidth="1"/>
-    <col min="9" max="9" width="24.8984375" style="12" customWidth="1"/>
-    <col min="10" max="10" width="13.796875" style="12" customWidth="1"/>
-    <col min="11" max="11" width="8.796875" style="12"/>
+    <col min="7" max="7" width="13" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="10" customWidth="1"/>
+    <col min="9" max="9" width="24.8984375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.796875" style="10" customWidth="1"/>
+    <col min="11" max="11" width="8.796875" style="10"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="3:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="3:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="3:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="18"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="5"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="3:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="3:11" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="13" t="s">
+      <c r="K20" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="3:11" ht="282" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="J21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="K21" s="11"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="3:11" ht="303.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K22" s="11"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>